<commit_message>
I made something. Tomorrow we'll find out if it works.
</commit_message>
<xml_diff>
--- a/lkoenig/Solar system info.xlsx
+++ b/lkoenig/Solar system info.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/23cf8e9ef9d770c3/Documents/my shit/School shit/Research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lak3r\Documents\GitHub\magicClassroom\lkoenig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{A89FEF06-2ED5-4F73-A474-28EE12024E15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{44F7E90C-B36E-4E6E-8785-1412ED440206}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D32142-E793-4F77-B11F-D31012DCC989}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="0" windowWidth="21600" windowHeight="12735" xr2:uid="{5465B1A2-3C2A-453E-9070-9B0FAEF0B2B0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{5465B1A2-3C2A-453E-9070-9B0FAEF0B2B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>Body</t>
   </si>
@@ -109,13 +109,46 @@
   </si>
   <si>
     <t>Small plannets scalled to earth and loage to jupiter</t>
+  </si>
+  <si>
+    <t>Currrent positions</t>
+  </si>
+  <si>
+    <t>(0,0,0)</t>
+  </si>
+  <si>
+    <t>(0,0,-0.75)</t>
+  </si>
+  <si>
+    <t>(0,0,-1)</t>
+  </si>
+  <si>
+    <t>(0,0,-1.6)</t>
+  </si>
+  <si>
+    <t>(0,0,-2)</t>
+  </si>
+  <si>
+    <t>(0,0,-3)</t>
+  </si>
+  <si>
+    <t>(0,0,-5)</t>
+  </si>
+  <si>
+    <t>(0,0,-6)</t>
+  </si>
+  <si>
+    <t>(0,0,-7)</t>
+  </si>
+  <si>
+    <t>(0,0,-8)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,12 +157,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -144,8 +183,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,13 +500,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E57B360-AD9E-4C60-810E-633DB3D5A081}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
@@ -478,7 +518,7 @@
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,7 +528,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -497,7 +537,7 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
@@ -519,7 +559,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -529,7 +569,7 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>0</v>
       </c>
       <c r="E2">
@@ -539,7 +579,7 @@
         <f>360/E2</f>
         <v>14.711892112791174</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <f>F2/5</f>
         <v>2.9423784225582348</v>
       </c>
@@ -565,7 +605,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -576,7 +616,7 @@
         <f>360/B3</f>
         <v>4.0927694406548438</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <f>C3/5</f>
         <v>0.81855388813096874</v>
       </c>
@@ -587,14 +627,14 @@
         <f t="shared" ref="F3:F12" si="0">360/E3</f>
         <v>6.1328790459965923</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <f t="shared" ref="G3:G12" si="1">F3/5</f>
         <v>1.2265758091993184</v>
       </c>
       <c r="H3">
         <v>2439.6999999999998</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <f t="shared" ref="I3:I12" si="2">(H3/6387)/4</f>
         <v>9.5494754971034906E-2</v>
       </c>
@@ -613,7 +653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -624,7 +664,7 @@
         <f t="shared" ref="C4:C12" si="5">360/B4</f>
         <v>1.6022787965105927</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <f t="shared" ref="D4:D12" si="6">C4/5</f>
         <v>0.32045575930211856</v>
       </c>
@@ -635,14 +675,14 @@
         <f t="shared" si="0"/>
         <v>1.4814814814814814</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <f t="shared" si="1"/>
         <v>0.29629629629629628</v>
       </c>
       <c r="H4">
         <v>6051.8</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="1">
         <f>(H4/6387)/4</f>
         <v>0.23687959918584625</v>
       </c>
@@ -661,7 +701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -672,7 +712,7 @@
         <f t="shared" si="5"/>
         <v>0.98559929912938726</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <f t="shared" si="6"/>
         <v>0.19711985982587746</v>
       </c>
@@ -683,14 +723,14 @@
         <f t="shared" si="0"/>
         <v>360</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
       <c r="H5">
         <v>6387</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="1">
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
@@ -709,7 +749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -720,7 +760,7 @@
         <f t="shared" si="5"/>
         <v>13.333333333333334</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <f t="shared" si="6"/>
         <v>2.666666666666667</v>
       </c>
@@ -731,7 +771,7 @@
         <f t="shared" si="0"/>
         <v>12.244897959183675</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <f t="shared" si="1"/>
         <v>2.4489795918367347</v>
       </c>
@@ -757,7 +797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -768,7 +808,7 @@
         <f t="shared" si="5"/>
         <v>0.52403272293225422</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <f t="shared" si="6"/>
         <v>0.10480654458645085</v>
       </c>
@@ -779,14 +819,14 @@
         <f t="shared" si="0"/>
         <v>350.87719298245611</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <f t="shared" si="1"/>
         <v>70.175438596491219</v>
       </c>
       <c r="H7">
         <v>3389.5</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="1">
         <f>(H7/6387)/4</f>
         <v>0.13267183341161734</v>
       </c>
@@ -805,7 +845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -817,7 +857,7 @@
         <f t="shared" si="5"/>
         <v>8.2191780821917804E-2</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <f t="shared" si="6"/>
         <v>1.643835616438356E-2</v>
       </c>
@@ -829,7 +869,7 @@
         <f t="shared" si="0"/>
         <v>878.04878048780495</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <f t="shared" si="1"/>
         <v>175.60975609756099</v>
       </c>
@@ -840,7 +880,7 @@
         <f t="shared" si="2"/>
         <v>2.7364568655080634</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="1">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -855,7 +895,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -867,7 +907,7 @@
         <f t="shared" si="5"/>
         <v>3.4010392064241848E-2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <f t="shared" si="6"/>
         <v>6.8020784128483697E-3</v>
       </c>
@@ -879,7 +919,7 @@
         <f t="shared" si="0"/>
         <v>847.05882352941182</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <f t="shared" si="1"/>
         <v>169.41176470588238</v>
       </c>
@@ -890,7 +930,7 @@
         <f t="shared" si="2"/>
         <v>2.2793173633943948</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="1">
         <f t="shared" si="3"/>
         <v>0.83294474403169749</v>
       </c>
@@ -905,7 +945,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -917,7 +957,7 @@
         <f t="shared" si="5"/>
         <v>1.1741682974559686E-2</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <f t="shared" si="6"/>
         <v>2.3483365949119373E-3</v>
       </c>
@@ -929,7 +969,7 @@
         <f t="shared" si="0"/>
         <v>482.68156424581014</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <f t="shared" si="1"/>
         <v>96.53631284916203</v>
       </c>
@@ -940,7 +980,7 @@
         <f t="shared" si="2"/>
         <v>0.99271958666040394</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="1">
         <f>H10/69911</f>
         <v>0.36277552888672743</v>
       </c>
@@ -955,7 +995,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -967,7 +1007,7 @@
         <f t="shared" si="5"/>
         <v>5.9775840597758407E-3</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <f t="shared" si="6"/>
         <v>1.1955168119551682E-3</v>
       </c>
@@ -979,7 +1019,7 @@
         <f t="shared" si="0"/>
         <v>452.35602094240835</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <f t="shared" si="1"/>
         <v>90.471204188481664</v>
       </c>
@@ -990,7 +1030,7 @@
         <f t="shared" si="2"/>
         <v>0.96375450133082829</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="1">
         <f t="shared" si="3"/>
         <v>0.35219064238817926</v>
       </c>
@@ -1005,7 +1045,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1017,7 +1057,7 @@
         <f t="shared" si="5"/>
         <v>3.9770216526734421E-3</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <f t="shared" si="6"/>
         <v>7.9540433053468837E-4</v>
       </c>
@@ -1028,14 +1068,14 @@
         <f t="shared" si="0"/>
         <v>56.338028169014088</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <f t="shared" si="1"/>
         <v>11.267605633802818</v>
       </c>
       <c r="H12">
         <v>1188.307</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="1">
         <f t="shared" si="2"/>
         <v>4.6512721152340696E-2</v>
       </c>
@@ -1054,12 +1094,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1068,6 +1108,97 @@
       </c>
       <c r="I15" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>